<commit_message>
Completed 11 features and ready to turn in
</commit_message>
<xml_diff>
--- a/Robbie_Robot_Shop_Scrum.xlsx
+++ b/Robbie_Robot_Shop_Scrum.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="175">
   <si>
     <t>Product Name:</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t>Create Robot Parts</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -936,11 +939,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="151527568"/>
-        <c:axId val="151528352"/>
+        <c:axId val="300201024"/>
+        <c:axId val="300201416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="151527568"/>
+        <c:axId val="300201024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +980,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="151528352"/>
+        <c:crossAx val="300201416"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +988,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151528352"/>
+        <c:axId val="300201416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1035,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="151527568"/>
+        <c:crossAx val="300201024"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1090,7 +1093,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1178,11 +1180,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="384624872"/>
-        <c:axId val="384625656"/>
+        <c:axId val="346127304"/>
+        <c:axId val="346130440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="384624872"/>
+        <c:axId val="346127304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1208,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -1219,7 +1220,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="384625656"/>
+        <c:crossAx val="346130440"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1227,7 +1228,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="384625656"/>
+        <c:axId val="346130440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1260,7 +1261,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1274,7 +1274,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="384624872"/>
+        <c:crossAx val="346127304"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1642,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2255,6 +2255,9 @@
       <c r="B38">
         <v>5</v>
       </c>
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
       <c r="E38" s="1">
         <v>1</v>
       </c>
@@ -2307,6 +2310,9 @@
       <c r="B40">
         <v>7</v>
       </c>
+      <c r="C40" t="s">
+        <v>147</v>
+      </c>
       <c r="E40" s="1">
         <v>1</v>
       </c>
@@ -2330,6 +2336,9 @@
       <c r="B41">
         <v>8</v>
       </c>
+      <c r="C41" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="E41" s="1">
         <v>1</v>
       </c>
@@ -2382,6 +2391,9 @@
       <c r="B43">
         <v>10</v>
       </c>
+      <c r="C43" t="s">
+        <v>147</v>
+      </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
@@ -2405,6 +2417,9 @@
       <c r="B44">
         <v>11</v>
       </c>
+      <c r="C44" t="s">
+        <v>147</v>
+      </c>
       <c r="E44" s="1">
         <v>1</v>
       </c>
@@ -2427,6 +2442,9 @@
       </c>
       <c r="B45">
         <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>147</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>

</xml_diff>